<commit_message>
added bot section to manifest added custom cache for dialog management fixes to recognize team/members if utterance has extra junk in it (i.e. <at>HuddleBot</at>
</commit_message>
<xml_diff>
--- a/Files/Teams.xlsx
+++ b/Files/Teams.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6188113-A563-489E-B15B-1DF45B26F67F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0895E818-FFD8-4EF8-9131-FB124F1CD40C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -49,13 +49,7 @@
     <t>Team 3</t>
   </si>
   <si>
-    <t>admin@M365x651745.onmicrosoft.com</t>
-  </si>
-  <si>
-    <t>AarifS@M365x651745.onmicrosoft.com</t>
-  </si>
-  <si>
-    <t>AarifS@M365x651745.onmicrosoft.com;AchimM@M365x651745.onmicrosoft.com</t>
+    <t>grjoh@jebosoft.onmicrosoft.com;tomjebo@jebosoft.onmicrosoft.com</t>
   </si>
 </sst>
 </file>
@@ -387,17 +381,17 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.46484375" customWidth="1"/>
-    <col min="4" max="4" width="67.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" customWidth="1"/>
+    <col min="4" max="4" width="67.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,7 +405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -422,10 +416,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -433,13 +427,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -449,6 +443,7 @@
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>